<commit_message>
Successfully uploads yearly reports.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/valerie_gutierrez_uipath_com/Documents/Documents/UiPath/GenerateYearlyReport for Vendor-REF-Performer/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{858A07BC-1A6B-4702-8ECE-B0EEDDBA2555}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B63FA49D-DD7C-46A2-A1B8-C6A8696E7E03}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40020" yWindow="2670" windowWidth="16485" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="51">
   <si>
     <t>Name</t>
   </si>
@@ -172,6 +172,12 @@
   </si>
   <si>
     <t>ACME_Credential</t>
+  </si>
+  <si>
+    <t>DownloadReports</t>
+  </si>
+  <si>
+    <t>Data\Temp</t>
   </si>
 </sst>
 </file>
@@ -557,7 +563,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -649,7 +655,14 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" t="s">
+        <v>50</v>
+      </c>
+    </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>